<commit_message>
Adaptation of script 'minimal.py' to be able to execute  multiple functions in a program
</commit_message>
<xml_diff>
--- a/ML/Results/Summary.xlsx
+++ b/ML/Results/Summary.xlsx
@@ -349,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -424,6 +424,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4709,7 +4713,7 @@
   <dimension ref="B1:R42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4972,140 +4976,140 @@
         <v>71.4989332720092</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
+    <row r="7" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="21" t="n">
         <f aca="false">AVERAGE(DT_M!B2:B100)</f>
         <v>76.1513486513486</v>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="22" t="n">
         <f aca="false">AVERAGE(DT_E!B4:B102)</f>
         <v>76.7803562308478</v>
       </c>
-      <c r="E7" s="21" t="n">
+      <c r="E7" s="22" t="n">
         <f aca="false">AVERAGE(kNN_M!B2:B100)</f>
         <v>70.4321928071928</v>
       </c>
-      <c r="F7" s="22" t="n">
+      <c r="F7" s="23" t="n">
         <f aca="false">AVERAGE(kNN_E!B2:B100)</f>
         <v>63.891438968335</v>
       </c>
-      <c r="G7" s="20" t="n">
+      <c r="G7" s="21" t="n">
         <f aca="false">AVERAGE(DT_M!C2:C100)</f>
         <v>75.1072394057442</v>
       </c>
-      <c r="H7" s="21" t="n">
+      <c r="H7" s="22" t="n">
         <f aca="false">AVERAGE(DT_E!C2:C100)</f>
         <v>76.3356103501361</v>
       </c>
-      <c r="I7" s="21" t="n">
+      <c r="I7" s="22" t="n">
         <f aca="false">AVERAGE(kNN_M!C2:C100)</f>
         <v>72.7856524191713</v>
       </c>
-      <c r="J7" s="22" t="n">
+      <c r="J7" s="23" t="n">
         <f aca="false">AVERAGE(kNN_E!C2:C100)</f>
         <v>63.895067700814</v>
       </c>
-      <c r="K7" s="20" t="n">
+      <c r="K7" s="21" t="n">
         <f aca="false">AVERAGE(DT_M!D2:D100)</f>
         <v>78.3399933399933</v>
       </c>
-      <c r="L7" s="21" t="n">
+      <c r="L7" s="22" t="n">
         <f aca="false">AVERAGE(DT_E!D2:D100)</f>
         <v>77.8700204290092</v>
       </c>
-      <c r="M7" s="21" t="n">
+      <c r="M7" s="22" t="n">
         <f aca="false">AVERAGE(kNN_M!D2:D100)</f>
         <v>65.9194971694972</v>
       </c>
-      <c r="N7" s="22" t="n">
+      <c r="N7" s="23" t="n">
         <f aca="false">AVERAGE(kNN_E!D2:D100)</f>
         <v>64.953013278856</v>
       </c>
-      <c r="O7" s="20" t="n">
+      <c r="O7" s="21" t="n">
         <f aca="false">AVERAGE(DT_M!E2:E100)</f>
         <v>76.7039805112611</v>
       </c>
-      <c r="P7" s="21" t="n">
+      <c r="P7" s="22" t="n">
         <f aca="false">AVERAGE(DT_E!E2:E100)</f>
         <v>76.8477599280408</v>
       </c>
-      <c r="Q7" s="21" t="n">
+      <c r="Q7" s="22" t="n">
         <f aca="false">AVERAGE(kNN_M!E2:E100)</f>
         <v>68.9337607017407</v>
       </c>
-      <c r="R7" s="22" t="n">
+      <c r="R7" s="23" t="n">
         <f aca="false">AVERAGE(kNN_E!E2:E100)</f>
         <v>64.1358622972391</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="24" t="n">
+      <c r="C8" s="25" t="n">
         <f aca="false">MEDIAN(DT_M!B2:B100)</f>
         <v>76.9921744921745</v>
       </c>
-      <c r="D8" s="25" t="n">
+      <c r="D8" s="26" t="n">
         <f aca="false">MEDIAN(DT_E!B5:B103)</f>
         <v>76.5104698672114</v>
       </c>
-      <c r="E8" s="25" t="n">
+      <c r="E8" s="26" t="n">
         <f aca="false">MEDIAN(kNN_M!B2:B100)</f>
         <v>70.5377955377955</v>
       </c>
-      <c r="F8" s="26" t="n">
+      <c r="F8" s="27" t="n">
         <f aca="false">MEDIAN(kNN_E!B2:B100)</f>
         <v>63.3203524004086</v>
       </c>
-      <c r="G8" s="24" t="n">
+      <c r="G8" s="25" t="n">
         <f aca="false">MEDIAN(DT_M!C2:C100)</f>
         <v>75.5788949857899</v>
       </c>
-      <c r="H8" s="25" t="n">
+      <c r="H8" s="26" t="n">
         <f aca="false">MEDIAN(DT_E!C2:C100)</f>
         <v>76.2900073317882</v>
       </c>
-      <c r="I8" s="25" t="n">
+      <c r="I8" s="26" t="n">
         <f aca="false">MEDIAN(kNN_M!C2:C100)</f>
         <v>73.0286853594589</v>
       </c>
-      <c r="J8" s="26" t="n">
+      <c r="J8" s="27" t="n">
         <f aca="false">MEDIAN(kNN_E!C2:C100)</f>
         <v>64.030784399852</v>
       </c>
-      <c r="K8" s="24" t="n">
+      <c r="K8" s="25" t="n">
         <f aca="false">MEDIAN(DT_M!D2:D100)</f>
         <v>78.8011988011988</v>
       </c>
-      <c r="L8" s="25" t="n">
+      <c r="L8" s="26" t="n">
         <f aca="false">MEDIAN(DT_E!D2:D100)</f>
         <v>77.3084780388151</v>
       </c>
-      <c r="M8" s="25" t="n">
+      <c r="M8" s="26" t="n">
         <f aca="false">MEDIAN(kNN_M!D2:D100)</f>
         <v>65.2430902430902</v>
       </c>
-      <c r="N8" s="26" t="n">
+      <c r="N8" s="27" t="n">
         <f aca="false">MEDIAN(kNN_E!D2:D100)</f>
         <v>64.1049540347293</v>
       </c>
-      <c r="O8" s="24" t="n">
+      <c r="O8" s="25" t="n">
         <f aca="false">MEDIAN(DT_M!E2:E100)</f>
         <v>76.9474142751016</v>
       </c>
-      <c r="P8" s="25" t="n">
+      <c r="P8" s="26" t="n">
         <f aca="false">MEDIAN(DT_E!E2:E100)</f>
         <v>76.7430372999957</v>
       </c>
-      <c r="Q8" s="25" t="n">
+      <c r="Q8" s="26" t="n">
         <f aca="false">MEDIAN(kNN_M!E2:E100)</f>
         <v>68.7369681188681</v>
       </c>
-      <c r="R8" s="26" t="n">
+      <c r="R8" s="27" t="n">
         <f aca="false">MEDIAN(kNN_E!E2:E100)</f>
         <v>62.7693423175577</v>
       </c>

</xml_diff>